<commit_message>
eDNA analysis final knitr
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/eDNA/3-Clean_data/ESV_higher_ANCOM_BC2.xlsx
+++ b/Multi-taxa_data/eDNA/3-Clean_data/ESV_higher_ANCOM_BC2.xlsx
@@ -417,14 +417,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Chattonellaceae</t>
+          <t>Order_Verongiida</t>
         </is>
       </c>
       <c r="B2">
-        <v>-4.202027131914781</v>
+        <v>-6.24020422541597</v>
       </c>
       <c r="C2">
-        <v>0.0005981729013846719</v>
+        <v>0.0001024706194922948</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -441,19 +441,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Class_Phaeophyceae</t>
+          <t>Order_Verongiida</t>
         </is>
       </c>
       <c r="B3">
-        <v>-5.097173032919231</v>
+        <v>8.839895652237658</v>
       </c>
       <c r="C3">
-        <v>2.646995896227074E-05</v>
+        <v>2.413483804509196E-06</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Impact
-low_vs_medium</t>
+medium_vs_high</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -465,14 +465,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Order_Verongiida</t>
+          <t>Petrosiidae</t>
         </is>
       </c>
       <c r="B4">
-        <v>-6.316932187754645</v>
+        <v>-5.487336006413498</v>
       </c>
       <c r="C4">
-        <v>8.77519903743495E-05</v>
+        <v>1.782639053368633E-05</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -489,19 +489,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Order_Verongiida</t>
+          <t>Chattonellaceae</t>
         </is>
       </c>
       <c r="B5">
-        <v>9.039249737060219</v>
+        <v>-4.093055456223142</v>
       </c>
       <c r="C5">
-        <v>1.8058661006867E-06</v>
+        <v>0.0008718637146058619</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>Impact
-medium_vs_high</t>
+low_vs_medium</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -513,14 +513,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Petrosiidae</t>
+          <t>Class_Phaeophyceae</t>
         </is>
       </c>
       <c r="B6">
-        <v>-5.588716839176056</v>
+        <v>-4.968706044194255</v>
       </c>
       <c r="C6">
-        <v>1.272002651661301E-05</v>
+        <v>4.254648742136053E-05</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -541,10 +541,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>4.609827896926669</v>
+        <v>4.618869259448249</v>
       </c>
       <c r="C7">
-        <v>0.000121221017220627</v>
+        <v>0.0001199447140529064</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -565,10 +565,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>6.239937742482658</v>
+        <v>6.289912686711788</v>
       </c>
       <c r="C8">
-        <v>2.203072927663875E-07</v>
+        <v>1.845403527087003E-07</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -589,10 +589,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>4.058540130558979</v>
+        <v>4.112657550358105</v>
       </c>
       <c r="C9">
-        <v>0.0008691238757966135</v>
+        <v>0.0007422452736906149</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>6.503056418092631</v>
+        <v>6.549253003326004</v>
       </c>
       <c r="C10">
-        <v>6.545942919138087E-07</v>
+        <v>5.784284659792789E-07</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -637,10 +637,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>7.078718382204198</v>
+        <v>7.110415739267379</v>
       </c>
       <c r="C11">
-        <v>5.56053423675714E-08</v>
+        <v>5.11252100811555E-08</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>-4.947757437490447</v>
+        <v>-4.951024750666711</v>
       </c>
       <c r="C12">
-        <v>5.544768728976908E-05</v>
+        <v>5.630960019763035E-05</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,10 +685,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>14.42248564434937</v>
+        <v>14.38946233558463</v>
       </c>
       <c r="C13">
-        <v>0.0001334600778626554</v>
+        <v>0.0001385368952025626</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -709,10 +709,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>15.0988862158211</v>
+        <v>14.97160525940761</v>
       </c>
       <c r="C14">
-        <v>0.0001296845741876891</v>
+        <v>0.0001381242253133509</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>

</xml_diff>